<commit_message>
optimiza solo una vez parametros e hiper parametros
</commit_message>
<xml_diff>
--- a/codigo_final_organizado/Simulaciones/lineal_estacionario/resultados_2_ESCENARIOS.xlsx
+++ b/codigo_final_organizado/Simulaciones/lineal_estacionario/resultados_2_ESCENARIOS.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N23"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -523,34 +523,34 @@
         <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.1871933284077594</v>
+        <v>-0.4391947799404573</v>
       </c>
       <c r="F2" t="n">
-        <v>0.6435510197032246</v>
+        <v>0.280176436088491</v>
       </c>
       <c r="G2" t="n">
-        <v>1.405352928587295</v>
+        <v>0.1427876977401354</v>
       </c>
       <c r="H2" t="n">
-        <v>0.400224350245707</v>
+        <v>0.4127792742118284</v>
       </c>
       <c r="I2" t="n">
-        <v>1.500619528091478</v>
+        <v>0.2052765787541329</v>
       </c>
       <c r="J2" t="n">
-        <v>1.208018199733981</v>
+        <v>1.253156790920255</v>
       </c>
       <c r="K2" t="n">
-        <v>1.927360641721842</v>
+        <v>0.2278851150392112</v>
       </c>
       <c r="L2" t="n">
-        <v>1.329544370917706</v>
+        <v>0.2459270742492109</v>
       </c>
       <c r="M2" t="n">
-        <v>1.567016812310027</v>
+        <v>0.3068672334673084</v>
       </c>
       <c r="N2" t="n">
-        <v>1.382851576616769</v>
+        <v>0.2544328657890937</v>
       </c>
     </row>
     <row r="3">
@@ -571,34 +571,34 @@
         <v>1</v>
       </c>
       <c r="E3" t="n">
-        <v>-1.702335400483121</v>
+        <v>-0.242712789843943</v>
       </c>
       <c r="F3" t="n">
-        <v>0.3564547265487462</v>
+        <v>0.2607050659720658</v>
       </c>
       <c r="G3" t="n">
-        <v>1.221782268137948</v>
+        <v>0.1536808083656432</v>
       </c>
       <c r="H3" t="n">
-        <v>0.7793319904649427</v>
+        <v>0.4089169444412364</v>
       </c>
       <c r="I3" t="n">
-        <v>1.381470890610097</v>
+        <v>0.2073276590729151</v>
       </c>
       <c r="J3" t="n">
-        <v>1.010420062794354</v>
+        <v>1.269323276420944</v>
       </c>
       <c r="K3" t="n">
-        <v>0.2137675238395462</v>
+        <v>0.2141025557800378</v>
       </c>
       <c r="L3" t="n">
-        <v>0.3434217885048705</v>
+        <v>0.161486837927117</v>
       </c>
       <c r="M3" t="n">
-        <v>1.467735954959121</v>
+        <v>0.2541949430787785</v>
       </c>
       <c r="N3" t="n">
-        <v>1.552278592054542</v>
+        <v>0.291707473161857</v>
       </c>
     </row>
     <row r="4">
@@ -619,34 +619,34 @@
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.6682738467366206</v>
+        <v>1.253050462133608</v>
       </c>
       <c r="F4" t="n">
-        <v>0.3388045843500642</v>
+        <v>0.9625195229041578</v>
       </c>
       <c r="G4" t="n">
-        <v>0.4356834413141638</v>
+        <v>0.6853251069471707</v>
       </c>
       <c r="H4" t="n">
-        <v>0.3956489306928614</v>
+        <v>1.077167118009555</v>
       </c>
       <c r="I4" t="n">
-        <v>0.6196120305860288</v>
+        <v>1.002848377288229</v>
       </c>
       <c r="J4" t="n">
-        <v>1.083692608393563</v>
+        <v>1.406145746643962</v>
       </c>
       <c r="K4" t="n">
-        <v>0.4836032102749406</v>
+        <v>1.233559888613904</v>
       </c>
       <c r="L4" t="n">
-        <v>0.9928564601806407</v>
+        <v>1.181711917024253</v>
       </c>
       <c r="M4" t="n">
-        <v>0.3332726571633392</v>
+        <v>0.9544738456940576</v>
       </c>
       <c r="N4" t="n">
-        <v>1.139317222032973</v>
+        <v>1.065505347579154</v>
       </c>
     </row>
     <row r="5">
@@ -667,34 +667,34 @@
         <v>1</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.9299716851858525</v>
+        <v>-1.43891302501105</v>
       </c>
       <c r="F5" t="n">
-        <v>0.1060555738798404</v>
+        <v>0.7290236225855294</v>
       </c>
       <c r="G5" t="n">
-        <v>0.621418703013853</v>
+        <v>2.225404221833818</v>
       </c>
       <c r="H5" t="n">
-        <v>0.466274410854165</v>
+        <v>0.6688286797701772</v>
       </c>
       <c r="I5" t="n">
-        <v>0.2712789391956478</v>
+        <v>2.434508968522655</v>
       </c>
       <c r="J5" t="n">
-        <v>1.061940671559081</v>
+        <v>1.162507405139005</v>
       </c>
       <c r="K5" t="n">
-        <v>0.6219857569024985</v>
+        <v>0.7094591483191943</v>
       </c>
       <c r="L5" t="n">
-        <v>0.2875786031082312</v>
+        <v>0.8873903387009525</v>
       </c>
       <c r="M5" t="n">
-        <v>0.7714809073792299</v>
+        <v>1.824927417794814</v>
       </c>
       <c r="N5" t="n">
-        <v>0.2402157589387164</v>
+        <v>2.140249381841854</v>
       </c>
     </row>
     <row r="6">
@@ -715,34 +715,34 @@
         <v>1</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.8982988624961146</v>
+        <v>-1.531871987019629</v>
       </c>
       <c r="F6" t="n">
-        <v>0.06971531556390434</v>
+        <v>0.7997529706806685</v>
       </c>
       <c r="G6" t="n">
-        <v>0.8097177071593051</v>
+        <v>0.2714281162697881</v>
       </c>
       <c r="H6" t="n">
-        <v>0.4691385764316047</v>
+        <v>0.6720338977700961</v>
       </c>
       <c r="I6" t="n">
-        <v>0.2109743028019812</v>
+        <v>0.15161754090967</v>
       </c>
       <c r="J6" t="n">
-        <v>1.057670873941617</v>
+        <v>1.157004304263798</v>
       </c>
       <c r="K6" t="n">
-        <v>0.2654317445511402</v>
+        <v>2.262738023745956</v>
       </c>
       <c r="L6" t="n">
-        <v>0.6003726168242929</v>
+        <v>2.502068556685275</v>
       </c>
       <c r="M6" t="n">
-        <v>0.8572634246951022</v>
+        <v>0.3433813703689279</v>
       </c>
       <c r="N6" t="n">
-        <v>0.4654770715384229</v>
+        <v>0.4895961622859197</v>
       </c>
     </row>
     <row r="7">
@@ -763,34 +763,34 @@
         <v>1</v>
       </c>
       <c r="E7" t="n">
-        <v>-1.861367486950452</v>
+        <v>-1.202172366945219</v>
       </c>
       <c r="F7" t="n">
-        <v>0.825490894905931</v>
+        <v>0.5781302272077913</v>
       </c>
       <c r="G7" t="n">
-        <v>1.595169121022683</v>
+        <v>0.3293385761621772</v>
       </c>
       <c r="H7" t="n">
-        <v>0.8939028290394717</v>
+        <v>0.606568683122727</v>
       </c>
       <c r="I7" t="n">
-        <v>0.5462451916678027</v>
+        <v>0.6196424600613908</v>
       </c>
       <c r="J7" t="n">
-        <v>0.9629093008993526</v>
+        <v>1.185519225601247</v>
       </c>
       <c r="K7" t="n">
-        <v>0.7028149148476075</v>
+        <v>0.3632176531356495</v>
       </c>
       <c r="L7" t="n">
-        <v>1.298077755070906</v>
+        <v>0.3022648373989401</v>
       </c>
       <c r="M7" t="n">
-        <v>1.800825790294419</v>
+        <v>0.3850827629145197</v>
       </c>
       <c r="N7" t="n">
-        <v>0.2688312726735941</v>
+        <v>0.2470106539886805</v>
       </c>
     </row>
     <row r="8">
@@ -811,34 +811,34 @@
         <v>1</v>
       </c>
       <c r="E8" t="n">
-        <v>-2.009686910611284</v>
+        <v>-0.7859611405635978</v>
       </c>
       <c r="F8" t="n">
-        <v>0.7391227962681665</v>
+        <v>0.3712384091483952</v>
       </c>
       <c r="G8" t="n">
-        <v>0.3092879844724303</v>
+        <v>0.2371940867112247</v>
       </c>
       <c r="H8" t="n">
-        <v>0.9437437318128993</v>
+        <v>0.4417492303824937</v>
       </c>
       <c r="I8" t="n">
-        <v>0.2199246535057888</v>
+        <v>0.2576599071762581</v>
       </c>
       <c r="J8" t="n">
-        <v>0.9500399769427612</v>
+        <v>1.221417944187562</v>
       </c>
       <c r="K8" t="n">
-        <v>0.5865845542165592</v>
+        <v>0.4618244738442552</v>
       </c>
       <c r="L8" t="n">
-        <v>1.147386288487255</v>
+        <v>0.404538414711585</v>
       </c>
       <c r="M8" t="n">
-        <v>0.3632784735524616</v>
+        <v>0.3086203908153451</v>
       </c>
       <c r="N8" t="n">
-        <v>0.224497742697541</v>
+        <v>0.2977671174255628</v>
       </c>
     </row>
     <row r="9">
@@ -859,34 +859,34 @@
         <v>1</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.5086736248511967</v>
+        <v>-1.079279607828528</v>
       </c>
       <c r="F9" t="n">
-        <v>0.6095129543808621</v>
+        <v>0.5051139283182715</v>
       </c>
       <c r="G9" t="n">
-        <v>1.231596960465284</v>
+        <v>0.8411596141356122</v>
       </c>
       <c r="H9" t="n">
-        <v>0.4060317916910545</v>
+        <v>0.5176588185280092</v>
       </c>
       <c r="I9" t="n">
-        <v>1.08295162643286</v>
+        <v>0.4460087325241173</v>
       </c>
       <c r="J9" t="n">
-        <v>1.124396484363874</v>
+        <v>1.195820114307767</v>
       </c>
       <c r="K9" t="n">
-        <v>0.755813477748167</v>
+        <v>0.2572519369261406</v>
       </c>
       <c r="L9" t="n">
-        <v>0.3463758014226903</v>
+        <v>0.3178307188154236</v>
       </c>
       <c r="M9" t="n">
-        <v>1.495011625570948</v>
+        <v>0.7445057657887683</v>
       </c>
       <c r="N9" t="n">
-        <v>0.5793670416871074</v>
+        <v>0.2334793241447689</v>
       </c>
     </row>
     <row r="10">
@@ -907,34 +907,34 @@
         <v>1</v>
       </c>
       <c r="E10" t="n">
-        <v>0.1248489796216299</v>
+        <v>-2.728073429524258</v>
       </c>
       <c r="F10" t="n">
-        <v>1.144980780110513</v>
+        <v>1.879263552013414</v>
       </c>
       <c r="G10" t="n">
-        <v>0.3597317723921675</v>
+        <v>1.796522250645631</v>
       </c>
       <c r="H10" t="n">
-        <v>0.4935608094505639</v>
+        <v>1.463981747179787</v>
       </c>
       <c r="I10" t="n">
-        <v>0.2858258093895247</v>
+        <v>1.136849246646469</v>
       </c>
       <c r="J10" t="n">
-        <v>1.092090401754291</v>
+        <v>1.123522395360715</v>
       </c>
       <c r="K10" t="n">
-        <v>1.439068791405507</v>
+        <v>1.303708147458225</v>
       </c>
       <c r="L10" t="n">
-        <v>0.8528038014558621</v>
+        <v>1.463847511456118</v>
       </c>
       <c r="M10" t="n">
-        <v>0.1681135209630868</v>
+        <v>1.758918002561617</v>
       </c>
       <c r="N10" t="n">
-        <v>0.5610847753959305</v>
+        <v>0.9907769132688189</v>
       </c>
     </row>
     <row r="11">
@@ -955,41 +955,39 @@
         <v>1</v>
       </c>
       <c r="E11" t="n">
-        <v>1.844675687069411</v>
+        <v>-2.127270602857722</v>
       </c>
       <c r="F11" t="n">
-        <v>2.569727506572614</v>
+        <v>1.29883550662934</v>
       </c>
       <c r="G11" t="n">
-        <v>0.511640526192328</v>
+        <v>0.3955541404947727</v>
       </c>
       <c r="H11" t="n">
-        <v>1.496159292579053</v>
+        <v>1.005200997856422</v>
       </c>
       <c r="I11" t="n">
-        <v>1.031548205554401</v>
+        <v>0.5478355534232571</v>
       </c>
       <c r="J11" t="n">
-        <v>1.516929164668523</v>
+        <v>1.115785822361156</v>
       </c>
       <c r="K11" t="n">
-        <v>1.554456333813129</v>
+        <v>0.700657162629562</v>
       </c>
       <c r="L11" t="n">
-        <v>0.955655116429022</v>
+        <v>0.8725883550636192</v>
       </c>
       <c r="M11" t="n">
-        <v>1.316583171666879</v>
+        <v>0.3737711421287407</v>
       </c>
       <c r="N11" t="n">
-        <v>0.6068945775348414</v>
+        <v>0.215932304366528</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Promedio</t>
-        </is>
+      <c r="A12" t="n">
+        <v>11</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -1004,134 +1002,136 @@
       <c r="D12" t="n">
         <v>1</v>
       </c>
-      <c r="E12" t="inlineStr"/>
+      <c r="E12" t="n">
+        <v>-0.1871933284077649</v>
+      </c>
       <c r="F12" t="n">
-        <v>0.7403416152283866</v>
+        <v>0.2526349897326587</v>
       </c>
       <c r="G12" t="n">
-        <v>0.8501381412757458</v>
+        <v>1.168452757981424</v>
       </c>
       <c r="H12" t="n">
-        <v>0.6744016713262324</v>
+        <v>0.4124235614055669</v>
       </c>
       <c r="I12" t="n">
-        <v>0.7150451177835609</v>
+        <v>1.517416636028743</v>
       </c>
       <c r="J12" t="n">
-        <v>1.10681077450514</v>
+        <v>1.275452209310847</v>
       </c>
       <c r="K12" t="n">
-        <v>0.8550886949320937</v>
+        <v>1.927360831597914</v>
       </c>
       <c r="L12" t="n">
-        <v>0.8154072602401475</v>
+        <v>1.950880463141911</v>
       </c>
       <c r="M12" t="n">
-        <v>1.014058233855461</v>
+        <v>1.049086563727598</v>
       </c>
       <c r="N12" t="n">
-        <v>0.7020815631170438</v>
+        <v>1.486144426923484</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>MA(1)</t>
+          <t>AR(1)</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>t-student</t>
+          <t>normal</t>
         </is>
       </c>
       <c r="D13" t="n">
         <v>1</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.8019825268384984</v>
+        <v>-1.702335400483126</v>
       </c>
       <c r="F13" t="n">
-        <v>0.2652639941168483</v>
+        <v>0.9202751044397484</v>
       </c>
       <c r="G13" t="n">
-        <v>0.2567453125547569</v>
+        <v>1.641422611303209</v>
       </c>
       <c r="H13" t="n">
-        <v>0.5360507557344912</v>
+        <v>0.7633635916933614</v>
       </c>
       <c r="I13" t="n">
-        <v>0.1923281788211045</v>
+        <v>1.71512473091498</v>
       </c>
       <c r="J13" t="n">
-        <v>0.8240690621055948</v>
+        <v>1.141763750330097</v>
       </c>
       <c r="K13" t="n">
-        <v>0.9149667824285264</v>
+        <v>0.2137678262991045</v>
       </c>
       <c r="L13" t="n">
-        <v>1.501559816234284</v>
+        <v>0.1621177730314299</v>
       </c>
       <c r="M13" t="n">
-        <v>0.2587080139253541</v>
+        <v>1.639879964488586</v>
       </c>
       <c r="N13" t="n">
-        <v>0.2126269518970051</v>
+        <v>1.573501925288991</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="n">
-        <v>2</v>
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Promedio</t>
+        </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>MA(1)</t>
+          <t>AR(1)</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>t-student</t>
+          <t>normal</t>
         </is>
       </c>
       <c r="D14" t="n">
         <v>1</v>
       </c>
-      <c r="E14" t="n">
-        <v>-2.205708600621761</v>
-      </c>
+      <c r="E14" t="inlineStr"/>
       <c r="F14" t="n">
-        <v>1.270069292907252</v>
+        <v>0.7364724446433776</v>
       </c>
       <c r="G14" t="n">
-        <v>1.250345599198468</v>
+        <v>0.8240224990492172</v>
       </c>
       <c r="H14" t="n">
-        <v>1.674968856754256</v>
+        <v>0.7042227120309383</v>
       </c>
       <c r="I14" t="n">
-        <v>1.870540481204931</v>
+        <v>0.8535096992769015</v>
       </c>
       <c r="J14" t="n">
-        <v>1.054802123027452</v>
+        <v>1.208951582070613</v>
       </c>
       <c r="K14" t="n">
-        <v>0.9367995334756044</v>
+        <v>0.8229610636157627</v>
       </c>
       <c r="L14" t="n">
-        <v>1.531633914500887</v>
+        <v>0.8710543998504864</v>
       </c>
       <c r="M14" t="n">
-        <v>1.627859209031492</v>
+        <v>0.8286424502357551</v>
       </c>
       <c r="N14" t="n">
-        <v>2.015915032732122</v>
+        <v>0.7738419913387261</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -1140,46 +1140,46 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>t-student</t>
+          <t>normal</t>
         </is>
       </c>
       <c r="D15" t="n">
         <v>1</v>
       </c>
       <c r="E15" t="n">
-        <v>-1.466761024637554</v>
+        <v>1.141401855113315</v>
       </c>
       <c r="F15" t="n">
-        <v>0.4453984482669353</v>
+        <v>0.5075510645285355</v>
       </c>
       <c r="G15" t="n">
-        <v>0.2761267593361629</v>
+        <v>0.4425270900194191</v>
       </c>
       <c r="H15" t="n">
-        <v>1.015402787487327</v>
+        <v>0.6873426639340973</v>
       </c>
       <c r="I15" t="n">
-        <v>0.205720811452432</v>
+        <v>0.480935467839805</v>
       </c>
       <c r="J15" t="n">
-        <v>0.8054504735710553</v>
+        <v>1.000960716553459</v>
       </c>
       <c r="K15" t="n">
-        <v>1.238168505420624</v>
+        <v>0.4137328462263857</v>
       </c>
       <c r="L15" t="n">
-        <v>1.857485154292868</v>
+        <v>0.3881190146688131</v>
       </c>
       <c r="M15" t="n">
-        <v>0.2727213816704854</v>
+        <v>0.48993745874591</v>
       </c>
       <c r="N15" t="n">
-        <v>0.3882142109306483</v>
+        <v>0.4171188928848244</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -1188,46 +1188,46 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>t-student</t>
+          <t>normal</t>
         </is>
       </c>
       <c r="D16" t="n">
         <v>1</v>
       </c>
       <c r="E16" t="n">
-        <v>-0.09044752041541054</v>
+        <v>0.7084844660375201</v>
       </c>
       <c r="F16" t="n">
-        <v>0.3652336085908607</v>
+        <v>0.2872389919768672</v>
       </c>
       <c r="G16" t="n">
-        <v>0.2938544007104754</v>
+        <v>0.3589553910411304</v>
       </c>
       <c r="H16" t="n">
-        <v>0.3154246606208368</v>
+        <v>0.4249238877321641</v>
       </c>
       <c r="I16" t="n">
-        <v>0.253885935618134</v>
+        <v>0.2791932327186922</v>
       </c>
       <c r="J16" t="n">
-        <v>0.8591078338921322</v>
+        <v>0.9690585179572595</v>
       </c>
       <c r="K16" t="n">
-        <v>1.427749966256307</v>
+        <v>0.3461926964689516</v>
       </c>
       <c r="L16" t="n">
-        <v>0.9246409695971591</v>
+        <v>0.2950962304401578</v>
       </c>
       <c r="M16" t="n">
-        <v>0.2464631572931303</v>
+        <v>0.3180726796419097</v>
       </c>
       <c r="N16" t="n">
-        <v>0.4172909589316178</v>
+        <v>0.2868960334512367</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -1236,46 +1236,46 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>t-student</t>
+          <t>normal</t>
         </is>
       </c>
       <c r="D17" t="n">
         <v>1</v>
       </c>
       <c r="E17" t="n">
-        <v>0.2718405741331466</v>
+        <v>1.229569142981684</v>
       </c>
       <c r="F17" t="n">
-        <v>0.5872808871844886</v>
+        <v>0.5628225057516014</v>
       </c>
       <c r="G17" t="n">
-        <v>0.3404242758919624</v>
+        <v>0.5827801375889246</v>
       </c>
       <c r="H17" t="n">
-        <v>0.3132645248173849</v>
+        <v>0.7203386850371382</v>
       </c>
       <c r="I17" t="n">
-        <v>0.2646503042985966</v>
+        <v>0.6615733798103053</v>
       </c>
       <c r="J17" t="n">
-        <v>0.9207527596882912</v>
+        <v>1.010476216589014</v>
       </c>
       <c r="K17" t="n">
-        <v>0.2285010444067438</v>
+        <v>0.4585608456823012</v>
       </c>
       <c r="L17" t="n">
-        <v>0.3458830219491964</v>
+        <v>0.3949615526122128</v>
       </c>
       <c r="M17" t="n">
-        <v>0.2554786659683662</v>
+        <v>0.8878256583226123</v>
       </c>
       <c r="N17" t="n">
-        <v>0.5891781040476418</v>
+        <v>0.5970703061922888</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -1284,46 +1284,46 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>t-student</t>
+          <t>normal</t>
         </is>
       </c>
       <c r="D18" t="n">
         <v>1</v>
       </c>
       <c r="E18" t="n">
-        <v>-0.152228760960047</v>
+        <v>0.03437408760461713</v>
       </c>
       <c r="F18" t="n">
-        <v>0.2781649641027136</v>
+        <v>0.2096391751375831</v>
       </c>
       <c r="G18" t="n">
-        <v>0.4669241104735672</v>
+        <v>0.0985937796770594</v>
       </c>
       <c r="H18" t="n">
-        <v>0.3091136806770108</v>
+        <v>0.2874921256625366</v>
       </c>
       <c r="I18" t="n">
-        <v>0.2753482778172471</v>
+        <v>0.3599808869973552</v>
       </c>
       <c r="J18" t="n">
-        <v>0.8617033624162962</v>
+        <v>0.934122833530018</v>
       </c>
       <c r="K18" t="n">
-        <v>0.2320460855571087</v>
+        <v>0.244534221575779</v>
       </c>
       <c r="L18" t="n">
-        <v>0.3052985126873261</v>
+        <v>0.203837593293866</v>
       </c>
       <c r="M18" t="n">
-        <v>0.357818248207625</v>
+        <v>0.2370117290626054</v>
       </c>
       <c r="N18" t="n">
-        <v>0.4500044462507475</v>
+        <v>0.2979527350847559</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -1332,46 +1332,46 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>t-student</t>
+          <t>normal</t>
         </is>
       </c>
       <c r="D19" t="n">
         <v>1</v>
       </c>
       <c r="E19" t="n">
-        <v>-0.2280437797829196</v>
+        <v>-0.7404453617352788</v>
       </c>
       <c r="F19" t="n">
-        <v>0.2250868861350368</v>
+        <v>0.7282435341770471</v>
       </c>
       <c r="G19" t="n">
-        <v>0.2886172519817137</v>
+        <v>0.2129165845899628</v>
       </c>
       <c r="H19" t="n">
-        <v>0.329127991048026</v>
+        <v>0.4590346201837199</v>
       </c>
       <c r="I19" t="n">
-        <v>0.2206319238617641</v>
+        <v>0.3541757538539416</v>
       </c>
       <c r="J19" t="n">
-        <v>0.8771403145596935</v>
+        <v>0.8937918814083594</v>
       </c>
       <c r="K19" t="n">
-        <v>0.2976681262247988</v>
+        <v>1.038307977717461</v>
       </c>
       <c r="L19" t="n">
-        <v>0.6810597607707589</v>
+        <v>1.309442047380737</v>
       </c>
       <c r="M19" t="n">
-        <v>0.2706106103654037</v>
+        <v>0.3339343028856485</v>
       </c>
       <c r="N19" t="n">
-        <v>0.2375378350211668</v>
+        <v>0.2722438403239087</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -1380,46 +1380,46 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>t-student</t>
+          <t>normal</t>
         </is>
       </c>
       <c r="D20" t="n">
         <v>1</v>
       </c>
       <c r="E20" t="n">
-        <v>-1.483469683252112</v>
+        <v>0.4771086536414199</v>
       </c>
       <c r="F20" t="n">
-        <v>0.5746292293126305</v>
+        <v>0.2111292732342254</v>
       </c>
       <c r="G20" t="n">
-        <v>1.25819038087649</v>
+        <v>0.5495615900826756</v>
       </c>
       <c r="H20" t="n">
-        <v>0.9528259118817614</v>
+        <v>0.3522665000503361</v>
       </c>
       <c r="I20" t="n">
-        <v>0.9037394318686953</v>
+        <v>0.3473352540062782</v>
       </c>
       <c r="J20" t="n">
-        <v>0.8126055669766704</v>
+        <v>0.9561192854715765</v>
       </c>
       <c r="K20" t="n">
-        <v>0.9289198257385639</v>
+        <v>0.5135814067064287</v>
       </c>
       <c r="L20" t="n">
-        <v>1.533043533112527</v>
+        <v>0.4425899763254381</v>
       </c>
       <c r="M20" t="n">
-        <v>0.5959357856092299</v>
+        <v>0.3057174417241412</v>
       </c>
       <c r="N20" t="n">
-        <v>1.238176922453013</v>
+        <v>0.5231268686430806</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -1428,137 +1428,329 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>t-student</t>
+          <t>normal</t>
         </is>
       </c>
       <c r="D21" t="n">
         <v>1</v>
       </c>
       <c r="E21" t="n">
-        <v>-0.786041425687011</v>
+        <v>-0.3463702240703861</v>
       </c>
       <c r="F21" t="n">
-        <v>0.1920945140926814</v>
+        <v>0.392092290394347</v>
       </c>
       <c r="G21" t="n">
-        <v>0.6630208342237706</v>
+        <v>0.5319515542583089</v>
       </c>
       <c r="H21" t="n">
-        <v>0.5210401327802625</v>
+        <v>0.3152596523709028</v>
       </c>
       <c r="I21" t="n">
-        <v>0.2730302987904711</v>
+        <v>0.5189697513727283</v>
       </c>
       <c r="J21" t="n">
-        <v>0.8245862935123677</v>
+        <v>0.9128258681411483</v>
       </c>
       <c r="K21" t="n">
-        <v>0.4290375719085924</v>
+        <v>0.2989946468868382</v>
       </c>
       <c r="L21" t="n">
-        <v>0.9076730420084533</v>
+        <v>0.2879082719847083</v>
       </c>
       <c r="M21" t="n">
-        <v>0.6815262751805425</v>
+        <v>0.8451301910767468</v>
       </c>
       <c r="N21" t="n">
-        <v>0.4691195656286929</v>
+        <v>0.6361884909149097</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
+        <v>8</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>MA(1)</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>1</v>
+      </c>
+      <c r="E22" t="n">
+        <v>-0.5026228807126156</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.514421596378396</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.3658970029212981</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.3709896675296706</v>
+      </c>
+      <c r="I22" t="n">
+        <v>0.2407201704327914</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0.9040373819525038</v>
+      </c>
+      <c r="K22" t="n">
+        <v>0.5990010350762384</v>
+      </c>
+      <c r="L22" t="n">
+        <v>0.7445187226335834</v>
+      </c>
+      <c r="M22" t="n">
+        <v>0.2405586025392189</v>
+      </c>
+      <c r="N22" t="n">
+        <v>0.2479343763128162</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>9</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>MA(1)</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>1</v>
+      </c>
+      <c r="E23" t="n">
+        <v>1.565371735592149</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.8105242011986641</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.8890083472707889</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.9970612799080135</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0.8117907682549476</v>
+      </c>
+      <c r="J23" t="n">
+        <v>1.072635371262174</v>
+      </c>
+      <c r="K23" t="n">
+        <v>1.459847285998825</v>
+      </c>
+      <c r="L23" t="n">
+        <v>1.467477504077702</v>
+      </c>
+      <c r="M23" t="n">
+        <v>1.128909287348441</v>
+      </c>
+      <c r="N23" t="n">
+        <v>1.020141639642666</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
         <v>10</v>
       </c>
-      <c r="B22" t="inlineStr">
+      <c r="B24" t="inlineStr">
         <is>
           <t>MA(1)</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>t-student</t>
-        </is>
-      </c>
-      <c r="D22" t="n">
-        <v>1</v>
-      </c>
-      <c r="E22" t="n">
-        <v>0.9378812871972964</v>
-      </c>
-      <c r="F22" t="n">
-        <v>1.254005367719575</v>
-      </c>
-      <c r="G22" t="n">
-        <v>0.7230227116237681</v>
-      </c>
-      <c r="H22" t="n">
-        <v>0.5479852209795467</v>
-      </c>
-      <c r="I22" t="n">
-        <v>0.4037483919711125</v>
-      </c>
-      <c r="J22" t="n">
-        <v>1.046182197213546</v>
-      </c>
-      <c r="K22" t="n">
-        <v>1.591763843102027</v>
-      </c>
-      <c r="L22" t="n">
-        <v>1.076588274434516</v>
-      </c>
-      <c r="M22" t="n">
-        <v>0.5196420492816607</v>
-      </c>
-      <c r="N22" t="n">
-        <v>0.3683056204477041</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>1</v>
+      </c>
+      <c r="E24" t="n">
+        <v>1.180199153518281</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.54396252000423</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.5120248111191985</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.6653250894237626</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0.3255266057257533</v>
+      </c>
+      <c r="J24" t="n">
+        <v>1.005552624703727</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0.6610368460343956</v>
+      </c>
+      <c r="L24" t="n">
+        <v>0.6412941475067608</v>
+      </c>
+      <c r="M24" t="n">
+        <v>0.4138564627361063</v>
+      </c>
+      <c r="N24" t="n">
+        <v>0.3394143072615533</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>11</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>MA(1)</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>1</v>
+      </c>
+      <c r="E25" t="n">
+        <v>-0.3955262208335694</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.4274531827696816</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0.2108172296920183</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0.338899223426163</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0.3302675841954401</v>
+      </c>
+      <c r="J25" t="n">
+        <v>0.9101282763350604</v>
+      </c>
+      <c r="K25" t="n">
+        <v>0.7617627807304622</v>
+      </c>
+      <c r="L25" t="n">
+        <v>0.9405715146724534</v>
+      </c>
+      <c r="M25" t="n">
+        <v>0.2935719918123803</v>
+      </c>
+      <c r="N25" t="n">
+        <v>0.2469574510428495</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>12</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>MA(1)</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>1</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.800713191375049</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.3283514969747308</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.4009704290249208</v>
+      </c>
+      <c r="H26" t="n">
+        <v>0.4603153074568959</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0.6599829845381477</v>
+      </c>
+      <c r="J26" t="n">
+        <v>0.9738749377081102</v>
+      </c>
+      <c r="K26" t="n">
+        <v>0.4502084755628941</v>
+      </c>
+      <c r="L26" t="n">
+        <v>0.3870530696538899</v>
+      </c>
+      <c r="M26" t="n">
+        <v>0.5545669212696475</v>
+      </c>
+      <c r="N26" t="n">
+        <v>0.6346492286616825</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
         <is>
           <t>Promedio</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
+      <c r="B27" t="inlineStr">
         <is>
           <t>MA(1)</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>t-student</t>
-        </is>
-      </c>
-      <c r="D23" t="n">
-        <v>1</v>
-      </c>
-      <c r="E23" t="inlineStr"/>
-      <c r="F23" t="n">
-        <v>0.5457227192429022</v>
-      </c>
-      <c r="G23" t="n">
-        <v>0.5817271636871135</v>
-      </c>
-      <c r="H23" t="n">
-        <v>0.6515204522780904</v>
-      </c>
-      <c r="I23" t="n">
-        <v>0.4863624035704488</v>
-      </c>
-      <c r="J23" t="n">
-        <v>0.8886399986963098</v>
-      </c>
-      <c r="K23" t="n">
-        <v>0.8225621284518898</v>
-      </c>
-      <c r="L23" t="n">
-        <v>1.066486599958797</v>
-      </c>
-      <c r="M23" t="n">
-        <v>0.5086763396533289</v>
-      </c>
-      <c r="N23" t="n">
-        <v>0.638636964834036</v>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>normal</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>1</v>
+      </c>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="n">
+        <v>0.4602858193771591</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0.4296669956071421</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0.5066040585596168</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0.4475376533121822</v>
+      </c>
+      <c r="J27" t="n">
+        <v>0.9619653259677009</v>
+      </c>
+      <c r="K27" t="n">
+        <v>0.60381342205558</v>
+      </c>
+      <c r="L27" t="n">
+        <v>0.6252391371041935</v>
+      </c>
+      <c r="M27" t="n">
+        <v>0.5040910605971139</v>
+      </c>
+      <c r="N27" t="n">
+        <v>0.4599745142013811</v>
       </c>
     </row>
   </sheetData>

</xml_diff>